<commit_message>
Improve doco, rename mass to body mass, add min & max trait values from ranges
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jim\uni\Papers and talks\Animal traits dbs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jim\uni\Papers and talks\AnimalTraits\animaltraits.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26820" windowHeight="10740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Column descriptions" sheetId="2" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Name of trait: mass/brain size/metabolic rate</t>
   </si>
   <si>
-    <t>Numeric trait value</t>
-  </si>
-  <si>
     <t>Required for metabolic rate measured as volume of CO2 production. Used to convert from CO2 production to the equivalent O2 consumption</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Free form text. Include text "DONTWARN" to exclude from QA high variability report</t>
+  </si>
+  <si>
+    <t>Numeric trait value or a range of values e.g. "5.3-8.9"</t>
   </si>
 </sst>
 </file>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,12 +1008,12 @@
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10"/>
     </row>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1110,7 +1110,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,7 +1134,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1158,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,7 +1166,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,20 +1182,20 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>